<commit_message>
modified the bug on Date
</commit_message>
<xml_diff>
--- a/now/eastmoney/eastmoney_lack.xlsx
+++ b/now/eastmoney/eastmoney_lack.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="12270"/>
+    <workbookView windowWidth="28785" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12434,8 +12434,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -12445,22 +12445,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12481,18 +12496,17 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -12504,6 +12518,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -12511,8 +12533,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12526,14 +12549,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -12542,7 +12557,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -12558,40 +12579,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -12604,25 +12604,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12634,13 +12628,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12652,13 +12646,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12676,7 +12676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12688,7 +12694,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12700,25 +12730,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12730,61 +12778,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12795,6 +12795,56 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -12816,67 +12866,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12895,151 +12886,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -13366,8 +13366,8 @@
   <sheetPr/>
   <dimension ref="A1:D3735"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2690" workbookViewId="0">
-      <selection activeCell="D2707" sqref="D2707"/>
+    <sheetView tabSelected="1" topLeftCell="A2656" workbookViewId="0">
+      <selection activeCell="D2662" sqref="D2662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -34645,12 +34645,15 @@
         <v>3010</v>
       </c>
     </row>
-    <row r="2662" spans="1:2">
+    <row r="2662" spans="1:4">
       <c r="A2662" t="s">
         <v>3019</v>
       </c>
       <c r="B2662" t="s">
         <v>3010</v>
+      </c>
+      <c r="D2662">
+        <v>12.28</v>
       </c>
     </row>
     <row r="2663" spans="1:2">

</xml_diff>